<commit_message>
Remove email column in importing grade form
</commit_message>
<xml_diff>
--- a/csv_files/ImportGrade.xlsx
+++ b/csv_files/ImportGrade.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NguyenKJ\Desktop\HK1 2023 2024\Web nâng cao\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\university\Web nâng cao\Final\csv_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31607CA8-9FCC-4CD6-95A1-FB291597F9FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33EF5AB1-FCBB-413C-9E64-3232BC437853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2205" yWindow="2205" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>Name</t>
   </si>
@@ -42,16 +42,10 @@
     <t>Student ID</t>
   </si>
   <si>
-    <t>Email</t>
-  </si>
-  <si>
     <t>First Name</t>
   </si>
   <si>
     <t>Last Name</t>
-  </si>
-  <si>
-    <t>abc@gmail.com</t>
   </si>
   <si>
     <t>A</t>
@@ -381,15 +375,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -397,7 +391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -405,7 +399,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -413,7 +407,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -424,52 +418,43 @@
         <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E5" t="s">
-        <v>2</v>
-      </c>
-      <c r="F5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>20120453</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="D6">
+        <v>10</v>
       </c>
       <c r="E6">
-        <v>10</v>
-      </c>
-      <c r="F6">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>20120454</v>
       </c>
       <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
         <v>8</v>
       </c>
-      <c r="C7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="D7">
         <v>10</v>
       </c>
       <c r="E7">
-        <v>10</v>
-      </c>
-      <c r="F7">
         <v>9</v>
       </c>
     </row>

</xml_diff>